<commit_message>
fix relationship for a couple of categories
</commit_message>
<xml_diff>
--- a/source-data/mappings/euklems-2018-isic4-to-fingreen-industry-map.xlsx
+++ b/source-data/mappings/euklems-2018-isic4-to-fingreen-industry-map.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="123">
   <si>
     <t xml:space="preserve">isic4</t>
   </si>
@@ -254,10 +254,10 @@
     <t xml:space="preserve">S95</t>
   </si>
   <si>
+    <t xml:space="preserve">ST</t>
+  </si>
+  <si>
     <t xml:space="preserve">T</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ST</t>
   </si>
   <si>
     <t xml:space="preserve">U</t>
@@ -683,10 +683,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="118" zoomScaleNormal="118" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -964,7 +964,7 @@
         <v>40</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="1"/>
@@ -977,7 +977,7 @@
         <v>41</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D24" s="7"/>
     </row>
@@ -1045,7 +1045,6 @@
       <c r="A30" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="0"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
     </row>
@@ -1151,7 +1150,6 @@
       <c r="A39" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B39" s="0"/>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
     </row>
@@ -1331,29 +1329,43 @@
       <c r="C54" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D54" s="7"/>
+      <c r="D54" s="7" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B55" s="6" t="s">
         <v>77</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>78</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D55" s="7"/>
+      <c r="D55" s="7" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B56" s="5"/>
-      <c r="C56" s="7"/>
-      <c r="D56" s="7"/>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="5"/>
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
     </row>
@@ -1404,6 +1416,10 @@
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C69" s="7"/>
       <c r="D69" s="7"/>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C70" s="7"/>
+      <c r="D70" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1759,7 +1775,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B42" s="13" t="s">
         <v>121</v>

</xml_diff>